<commit_message>
Authorization service find group of role.
</commit_message>
<xml_diff>
--- a/sdk/sdk-resources/com/constellio/app/services/schemas/bulkImport/data/excel/Excel2007FileImportDataIteratorAcceptanceTest-data.xlsx
+++ b/sdk/sdk-resources/com/constellio/app/services/schemas/bulkImport/data/excel/Excel2007FileImportDataIteratorAcceptanceTest-data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Constellio\constellio\sdk\sdk-resources\com\constellio\app\services\schemas\bulkImport\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\constellios\Documents\constellio3-Copie\constellio\sdk\sdk-resources\com\constellio\app\services\schemas\bulkImport\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B912D3-EAF3-47F0-B613-B2AED1F4E558}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="622"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="622" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datas-exception" sheetId="4" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="34">
   <si>
     <t>schema</t>
   </si>
@@ -162,11 +163,20 @@
   <si>
     <t>anotherCustomSchema</t>
   </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>8-10</t>
+  </si>
+  <si>
+    <t>10-9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -200,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -210,6 +220,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,18 +585,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="17.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="88" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -617,7 +630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -637,7 +650,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>42</v>
       </c>
@@ -648,7 +661,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -671,13 +684,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>22</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="7"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -691,18 +707,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="17.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="88" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -734,7 +753,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -754,7 +773,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>42</v>
       </c>
@@ -765,7 +784,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -786,6 +805,19 @@
       </c>
       <c r="J5" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -800,18 +832,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="61.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -843,7 +875,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -860,7 +892,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -883,12 +915,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -920,14 +952,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:12" ht="102" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -962,7 +994,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -982,7 +1014,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1008,7 +1040,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1026,7 +1058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Excel option : importAsLegacyId
</commit_message>
<xml_diff>
--- a/sdk/sdk-resources/com/constellio/app/services/schemas/bulkImport/data/excel/Excel2007FileImportDataIteratorAcceptanceTest-data.xlsx
+++ b/sdk/sdk-resources/com/constellio/app/services/schemas/bulkImport/data/excel/Excel2007FileImportDataIteratorAcceptanceTest-data.xlsx
@@ -1,29 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\constellios\Documents\constellio3-Copie\constellio\sdk\sdk-resources\com\constellio\app\services\schemas\bulkImport\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\dev-constellio-java8\constellio\sdk\sdk-resources\com\constellio\app\services\schemas\bulkImport\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B912D3-EAF3-47F0-B613-B2AED1F4E558}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C6F9F5-5DA3-4BD8-9CD6-3A1F420AF4E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="622" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="622" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datas-exception" sheetId="4" r:id="rId1"/>
-    <sheet name="datas" sheetId="1" r:id="rId2"/>
-    <sheet name="content" sheetId="2" r:id="rId3"/>
-    <sheet name="dates" sheetId="3" r:id="rId4"/>
+    <sheet name="option-importAsLegacyId-false" sheetId="6" r:id="rId2"/>
+    <sheet name="option-importAsLegacyId-true" sheetId="5" r:id="rId3"/>
+    <sheet name="datas" sheetId="1" r:id="rId4"/>
+    <sheet name="content" sheetId="2" r:id="rId5"/>
+    <sheet name="dates" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="40">
   <si>
     <t>schema</t>
   </si>
@@ -171,6 +173,26 @@
   </si>
   <si>
     <t>10-9</t>
+  </si>
+  <si>
+    <t>id
+importAsLegacyId=true</t>
+  </si>
+  <si>
+    <t>id
+importAsLegacyId=false</t>
+  </si>
+  <si>
+    <t>000042</t>
+  </si>
+  <si>
+    <t>000666</t>
+  </si>
+  <si>
+    <t>000032</t>
+  </si>
+  <si>
+    <t>000001</t>
   </si>
 </sst>
 </file>
@@ -210,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -221,6 +243,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,13 +619,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="93" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -630,7 +657,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -650,7 +677,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>42</v>
       </c>
@@ -661,7 +688,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -684,7 +711,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>22</v>
       </c>
@@ -692,7 +719,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
     </row>
   </sheetData>
@@ -707,26 +734,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8DF1F1-D392-4750-B661-2009CB363B29}">
+  <dimension ref="A2:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="93" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="B2" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -753,12 +780,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -773,9 +800,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4">
-        <v>42</v>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -784,12 +811,12 @@
         <v>666</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
-        <v>666</v>
+      <c r="B5" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -807,17 +834,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
-        <v>31</v>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -832,18 +854,268 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85A1341-E3A5-47DB-B78C-2DD7B79364B3}">
+  <dimension ref="A2:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" ht="93" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>666</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" ht="93" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>666</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -875,7 +1147,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -892,7 +1164,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -915,12 +1187,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -951,15 +1223,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="108" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -994,7 +1266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1014,7 +1286,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1040,7 +1312,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1058,7 +1330,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Excel option : importAsLegacyId=true/false for Java 7
</commit_message>
<xml_diff>
--- a/sdk/sdk-resources/com/constellio/app/services/schemas/bulkImport/data/excel/Excel2007FileImportDataIteratorAcceptanceTest-data.xlsx
+++ b/sdk/sdk-resources/com/constellio/app/services/schemas/bulkImport/data/excel/Excel2007FileImportDataIteratorAcceptanceTest-data.xlsx
@@ -1,29 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\constellios\Documents\constellio3-Copie\constellio\sdk\sdk-resources\com\constellio\app\services\schemas\bulkImport\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\dev-constellio-java7\constellio\sdk\sdk-resources\com\constellio\app\services\schemas\bulkImport\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B912D3-EAF3-47F0-B613-B2AED1F4E558}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FAA4C0-D1D8-477A-BE50-BB596A712516}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="622" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="622" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datas-exception" sheetId="4" r:id="rId1"/>
-    <sheet name="datas" sheetId="1" r:id="rId2"/>
-    <sheet name="content" sheetId="2" r:id="rId3"/>
-    <sheet name="dates" sheetId="3" r:id="rId4"/>
+    <sheet name="option-importAsLegacyId-false" sheetId="6" r:id="rId2"/>
+    <sheet name="option-importAsLegacyId-true" sheetId="5" r:id="rId3"/>
+    <sheet name="datas" sheetId="1" r:id="rId4"/>
+    <sheet name="content" sheetId="2" r:id="rId5"/>
+    <sheet name="dates" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="41">
   <si>
     <t>schema</t>
   </si>
@@ -171,6 +173,29 @@
   </si>
   <si>
     <t>10-9</t>
+  </si>
+  <si>
+    <t>id
+importAsLegacyId=true</t>
+  </si>
+  <si>
+    <t>id
+importAsLegacyId=false</t>
+  </si>
+  <si>
+    <t>00000001</t>
+  </si>
+  <si>
+    <t>00000042</t>
+  </si>
+  <si>
+    <t>00000666</t>
+  </si>
+  <si>
+    <t>00000032</t>
+  </si>
+  <si>
+    <t>00000810</t>
   </si>
 </sst>
 </file>
@@ -210,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -221,6 +246,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,13 +622,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="93" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -630,7 +660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -650,7 +680,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>42</v>
       </c>
@@ -661,7 +691,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -684,7 +714,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>22</v>
       </c>
@@ -692,7 +722,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
     </row>
   </sheetData>
@@ -707,26 +737,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1927D3-7388-4576-BD3C-7F9649B3F7E6}">
   <dimension ref="A2:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="93" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="B2" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -753,12 +783,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -773,9 +803,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4">
-        <v>42</v>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -784,12 +814,12 @@
         <v>666</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
-        <v>666</v>
+      <c r="B5" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -807,17 +837,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
-        <v>31</v>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
-        <v>32</v>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -832,18 +862,268 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81406A4D-257A-4A90-AB93-584CB366C26F}">
+  <dimension ref="A2:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" ht="93" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>666</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" ht="93" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>666</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -875,7 +1155,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -892,7 +1172,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -915,12 +1195,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -951,15 +1231,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="108" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -994,7 +1274,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1014,7 +1294,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1040,7 +1320,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1058,7 +1338,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>

</xml_diff>